<commit_message>
kind of working in full with dynamic title selector
</commit_message>
<xml_diff>
--- a/carousell_listings.xlsx
+++ b/carousell_listings.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H340"/>
+  <dimension ref="A1:H345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
       <selection activeCell="A184" sqref="A183:XFD184"/>
@@ -14700,6 +14700,216 @@
         </is>
       </c>
     </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1313409423</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>https://www.carousell.sg/p/1313409423</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>little_stiches</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>Apple Pencil Gen 1 (Free case)</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>S$80</t>
+        </is>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>Like new</t>
+        </is>
+      </c>
+      <c r="H341" t="inlineStr">
+        <is>
+          <t>https://media.karousell.com/media/photos/products/2024/7/9/apple_pencil_gen_1_free_case_1720547160_018d4006_progressive_thumbnail.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1313128588</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>https://www.carousell.sg/p/1313128588</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>zaw_m_h</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>Apple Pencil Gen 1</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>S$110</t>
+        </is>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>Lightly used</t>
+        </is>
+      </c>
+      <c r="H342" t="inlineStr">
+        <is>
+          <t>https://media.karousell.com/media/photos/products/2024/7/8/apple_pencil_gen_1_1720430285_84c0e654_progressive_thumbnail.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1312992098</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>https://www.carousell.sg/p/1312992098</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>heartaimer</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>Apple Pencil Gen 1</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>S$75</t>
+        </is>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>Like new</t>
+        </is>
+      </c>
+      <c r="H343" t="inlineStr">
+        <is>
+          <t>https://media.karousell.com/media/photos/products/2024/7/7/apple_pencil_gen_1_1720362436_2b2d690f_progressive_thumbnail.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1312916504</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>https://www.carousell.sg/p/1312916504</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>auzra35</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>Apple Pencil Gen 1</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>S$90</t>
+        </is>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>Like new</t>
+        </is>
+      </c>
+      <c r="H344" t="inlineStr">
+        <is>
+          <t>https://media.karousell.com/media/photos/products/2024/7/7/apple_pencil_gen_1_1720340083_9423c6b1_progressive_thumbnail.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1312513290</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>https://www.carousell.sg/p/1312513290</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>yljc199702018</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>Apple Pencil Gen 1</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>S$100</t>
+        </is>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>Like new</t>
+        </is>
+      </c>
+      <c r="H345" t="inlineStr">
+        <is>
+          <t>https://media.karousell.com/media/photos/products/2024/7/5/apple_pencil_gen_1_1720157937_2fe922b0_progressive_thumbnail.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>